<commit_message>
docs: Modifying api files
</commit_message>
<xml_diff>
--- a/api/Board/Board_API.xlsx
+++ b/api/Board/Board_API.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Documents\GitHub\AISW_Web_Community\api\Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D745DCCB-78FE-47E9-8719-8C904EEF6779}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76949C75-5C28-436A-B510-A756D7E6CE45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4D31F6B6-070E-4774-AAEF-202F9D53FBBB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t>Title</t>
   </si>
@@ -348,8 +348,8 @@
         <family val="2"/>
       </rPr>
       <t>",
-      "category" : "FREE",
-      "attachment_file" : "/User/notice.docx",
+      "category" : "UNIVERSITY",
+      "status" : "URGENT".
       "created_by" : "Hong gil dong",
       "created_at" : "2021-01-01T01:01:11.111",
       "views" : 1
@@ -364,12 +364,136 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>상태</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <r>
+      <t>URGENT(긴급</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 0, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t>TOP(상단</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t>고정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t>GENERAL(일반</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,6 +582,20 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="돋움"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="8">
@@ -573,7 +711,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -627,34 +765,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -664,6 +787,27 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -982,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B60143-E3B9-4AB4-9B51-6040CE152FCC}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -998,95 +1142,95 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -1135,64 +1279,64 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="35"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
@@ -1332,11 +1476,11 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="8"/>
@@ -1344,19 +1488,19 @@
         <v>35</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A24" s="9" t="s">
-        <v>41</v>
+      <c r="A24" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="8"/>
@@ -1366,83 +1510,93 @@
       <c r="G24" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="H24" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" s="9" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A25" s="21" t="s">
-        <v>44</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A26" s="21" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A26" s="9" t="s">
-        <v>46</v>
-      </c>
       <c r="B26" s="8"/>
-      <c r="C26" s="9" t="s">
-        <v>47</v>
+      <c r="C26" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="8"/>
-      <c r="F26" s="9" t="s">
+      <c r="F26" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A27" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G27" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H26" s="9" t="s">
+      <c r="H27" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A27" s="28" t="s">
+    <row r="28" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
-    </row>
-    <row r="28" spans="1:8" ht="312.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="31" t="s">
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="25"/>
+    </row>
+    <row r="29" spans="1:8" ht="305.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A29" s="20"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="38"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="20"/>
@@ -2047,7 +2201,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
     <mergeCell ref="A28:H28"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="A11:H11"/>
@@ -2055,12 +2215,6 @@
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="B15:H15"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
docs: Adding writer in api files
</commit_message>
<xml_diff>
--- a/api/Board/Board_API.xlsx
+++ b/api/Board/Board_API.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Documents\GitHub\AISW_Web_Community\api\Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9527583F-26DD-4B31-B652-FA48647BEE5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D452D3-6019-4D34-87C0-167B6F9EAF8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4D31F6B6-070E-4774-AAEF-202F9D53FBBB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4D31F6B6-070E-4774-AAEF-202F9D53FBBB}"/>
   </bookViews>
   <sheets>
     <sheet name="게시판 전체 조회" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="70">
   <si>
     <t>Title</t>
   </si>
@@ -187,10 +187,6 @@
   </si>
   <si>
     <t>작성자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>created_by</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -299,6 +295,374 @@
   </si>
   <si>
     <t>FREE / QNA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상태</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <r>
+      <t>URGENT(긴급</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 0, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t>TOP(상단</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t>고정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t>GENERAL(일반</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pagination </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>부</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>전체</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>페이지</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total_pages</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>전체</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>아이템</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total_elements</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>현재</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>페이지</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>current_page</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>현재</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>페이지</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>아이템</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>current_elements</t>
+  </si>
+  <si>
+    <t>default 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>생성일자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>writer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -350,7 +714,7 @@
       <t>",
       "category" : "UNIVERSITY",
       "status" : "URGENT".
-      "created_by" : "Hong gil dong",
+      "writer" : "Hong gil dong",
       "created_at" : "2021-01-01T01:01:11.111",
       "views" : 1
    }],
@@ -362,366 +726,6 @@
    }
 }</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상태</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <r>
-      <t>URGENT(긴급</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 0, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="3"/>
-      </rPr>
-      <t>TOP(상단</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="3"/>
-      </rPr>
-      <t>고정</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">1, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="3"/>
-      </rPr>
-      <t>GENERAL(일반</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Pagination </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>부</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>전체</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>페이지</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>수</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>total_pages</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>전체</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>아이템</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>수</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>total_elements</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>현재</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>페이지</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>current_page</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>현재</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>페이지</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>아이템</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>수</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>current_elements</t>
-  </si>
-  <si>
-    <t>default 10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1014,6 +1018,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1036,15 +1046,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1058,10 +1059,13 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1381,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B60143-E3B9-4AB4-9B51-6040CE152FCC}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1397,95 +1401,95 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
+      <c r="B3" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -1534,64 +1538,64 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
+      <c r="A12" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="36"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
@@ -1691,7 +1695,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
@@ -1706,7 +1710,7 @@
         <v>19</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
@@ -1731,11 +1735,11 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="8"/>
@@ -1746,7 +1750,7 @@
         <v>19</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
@@ -1766,7 +1770,7 @@
         <v>40</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
@@ -1775,7 +1779,7 @@
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="8"/>
@@ -1791,47 +1795,47 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="19" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>40</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="8"/>
       <c r="F27" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>40</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
@@ -1843,11 +1847,11 @@
     </row>
     <row r="29" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B29" s="20"/>
-      <c r="C29" s="38" t="s">
-        <v>61</v>
+      <c r="C29" s="22" t="s">
+        <v>59</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
@@ -1857,15 +1861,15 @@
       <c r="G29" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H29" s="38"/>
+      <c r="H29" s="22"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B30" s="20"/>
-      <c r="C30" s="39" t="s">
-        <v>63</v>
+      <c r="C30" s="23" t="s">
+        <v>61</v>
       </c>
       <c r="D30" s="20"/>
       <c r="E30" s="20"/>
@@ -1875,15 +1879,15 @@
       <c r="G30" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H30" s="38"/>
+      <c r="H30" s="22"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B31" s="20"/>
-      <c r="C31" s="39" t="s">
-        <v>65</v>
+      <c r="C31" s="23" t="s">
+        <v>63</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
@@ -1893,15 +1897,15 @@
       <c r="G31" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H31" s="38"/>
+      <c r="H31" s="22"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B32" s="20"/>
-      <c r="C32" s="39" t="s">
-        <v>67</v>
+      <c r="C32" s="23" t="s">
+        <v>65</v>
       </c>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
@@ -1911,33 +1915,33 @@
       <c r="G32" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H32" s="38" t="s">
-        <v>68</v>
+      <c r="H32" s="22" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="32"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="39"/>
     </row>
     <row r="34" spans="1:8" ht="324" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="24"/>
+      <c r="A34" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="26"/>
     </row>
     <row r="35" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="36" spans="1:8" ht="367.5" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>